<commit_message>
Updated data and metadata files to correct typos and match paper.
</commit_message>
<xml_diff>
--- a/Data and Metadata Files/chemical_metadata.xlsx
+++ b/Data and Metadata Files/chemical_metadata.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/jdprest_emory_edu/Documents/Research/Manuscripts and Projects/Active Projects/Thyroid Exposomics Paper/MANUSCRIPT SUBMISSIONS/Thyroid Lancet/Supplementary Construction/thyroid-exposomics-2025/Data and Metadata Files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emory-my.sharepoint.com/personal/jdprest_emory_edu/Documents/Research/Manuscripts and Projects/Active Projects/Thyroid Exposomics Paper/MANUSCRIPT SUBMISSIONS/Thyroid Lancet/thyroid-exposomics-2025/Data and Metadata Files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1189" documentId="8_{B4A3A8FD-2D75-4F4E-8AE7-7CB7BA630849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F16A9A3F-3AFB-0646-A516-D20F8F662059}"/>
+  <xr:revisionPtr revIDLastSave="1190" documentId="8_{B4A3A8FD-2D75-4F4E-8AE7-7CB7BA630849}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30CEA8E5-4A3F-E348-B2E6-4AAEFA9A727A}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="30240" windowHeight="18900" xr2:uid="{3C529916-AEB2-5A4C-9AEE-70179AF9DBE7}"/>
   </bookViews>
@@ -11512,9 +11512,6 @@
     <t>O,O-Diethyl phosphonate</t>
   </si>
   <si>
-    <t xml:space="preserve">Occtyl-Methoxycinnamate </t>
-  </si>
-  <si>
     <t xml:space="preserve">p-Dimethylaminoazobenzene </t>
   </si>
   <si>
@@ -11750,6 +11747,9 @@
   </si>
   <si>
     <t>γ-BHC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">octyl-Methoxycinnamate </t>
   </si>
 </sst>
 </file>
@@ -11859,7 +11859,7 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -12291,7 +12291,7 @@
   <dimension ref="A1:AD444"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A55" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
-      <selection activeCell="C78" sqref="C78"/>
+      <selection activeCell="E61" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12422,7 +12422,7 @@
         <v>105</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>3878</v>
+        <v>3877</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>3069</v>
@@ -12506,7 +12506,7 @@
         <v>105</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>3879</v>
+        <v>3878</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>694</v>
@@ -12586,7 +12586,7 @@
         <v>105</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>3880</v>
+        <v>3879</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>848</v>
@@ -12668,7 +12668,7 @@
         <v>105</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>3881</v>
+        <v>3880</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2680</v>
@@ -12748,10 +12748,10 @@
         <v>105</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>2764</v>
@@ -12828,10 +12828,10 @@
         <v>105</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>2764</v>
@@ -12910,10 +12910,10 @@
         <v>105</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>3884</v>
+        <v>3883</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>2764</v>
@@ -17685,7 +17685,7 @@
         <v>866</v>
       </c>
       <c r="D68" s="2" t="s">
-        <v>3897</v>
+        <v>3896</v>
       </c>
       <c r="E68" s="2" t="s">
         <v>865</v>
@@ -19588,10 +19588,10 @@
         <v>105</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>3851</v>
+        <v>3850</v>
       </c>
       <c r="D92" s="2" t="s">
-        <v>3851</v>
+        <v>3850</v>
       </c>
       <c r="E92" s="2" t="s">
         <v>778</v>
@@ -19670,7 +19670,7 @@
         <v>105</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>3854</v>
+        <v>3853</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>772</v>
@@ -23427,12 +23427,12 @@
         <v>125</v>
       </c>
       <c r="T140" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="U140" s="2"/>
       <c r="V140" s="2"/>
       <c r="W140" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="X140" s="2" t="s">
         <v>92</v>
@@ -23620,7 +23620,7 @@
         <v>1</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>3825</v>
+        <v>3824</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>2379</v>
@@ -23778,10 +23778,10 @@
         <v>105</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
       <c r="D145" s="2" t="s">
-        <v>3848</v>
+        <v>3847</v>
       </c>
       <c r="E145" s="2" t="s">
         <v>2612</v>
@@ -23856,7 +23856,7 @@
         <v>105</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>3849</v>
+        <v>3848</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>466</v>
@@ -24014,10 +24014,10 @@
         <v>105</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>3853</v>
+        <v>3852</v>
       </c>
       <c r="D148" s="2" t="s">
-        <v>3853</v>
+        <v>3852</v>
       </c>
       <c r="E148" s="2" t="s">
         <v>814</v>
@@ -26630,7 +26630,7 @@
         <v>105</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>237</v>
@@ -26708,10 +26708,10 @@
         <v>105</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="D182" s="2" t="s">
-        <v>3846</v>
+        <v>3845</v>
       </c>
       <c r="E182" s="2" t="s">
         <v>920</v>
@@ -27412,7 +27412,7 @@
         <v>105</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>2322</v>
@@ -27642,10 +27642,10 @@
         <v>105</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="D194" s="2" t="s">
-        <v>3889</v>
+        <v>3888</v>
       </c>
       <c r="E194" s="2" t="s">
         <v>3468</v>
@@ -28664,7 +28664,7 @@
         <v>105</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>3828</v>
+        <v>3827</v>
       </c>
       <c r="D207" s="2" t="s">
         <v>418</v>
@@ -28820,10 +28820,10 @@
         <v>105</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="D209" s="2" t="s">
-        <v>3842</v>
+        <v>3841</v>
       </c>
       <c r="E209" s="2" t="s">
         <v>1298</v>
@@ -29446,10 +29446,10 @@
         <v>105</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>3874</v>
+        <v>3873</v>
       </c>
       <c r="D217" s="2" t="s">
-        <v>3874</v>
+        <v>3873</v>
       </c>
       <c r="E217" s="2" t="s">
         <v>544</v>
@@ -29530,10 +29530,10 @@
         <v>105</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>3875</v>
+        <v>3874</v>
       </c>
       <c r="D218" s="2" t="s">
-        <v>3875</v>
+        <v>3874</v>
       </c>
       <c r="E218" s="2" t="s">
         <v>1836</v>
@@ -32188,7 +32188,7 @@
         <v>105</v>
       </c>
       <c r="C252" s="2" t="s">
-        <v>3864</v>
+        <v>3863</v>
       </c>
       <c r="D252" s="2" t="s">
         <v>2597</v>
@@ -32896,7 +32896,7 @@
         <v>105</v>
       </c>
       <c r="C261" s="2" t="s">
-        <v>3833</v>
+        <v>3832</v>
       </c>
       <c r="D261" s="2" t="s">
         <v>3009</v>
@@ -34228,10 +34228,10 @@
         <v>105</v>
       </c>
       <c r="C278" s="2" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="D278" s="2" t="s">
-        <v>3856</v>
+        <v>3855</v>
       </c>
       <c r="E278" s="2" t="s">
         <v>627</v>
@@ -34702,10 +34702,10 @@
         <v>105</v>
       </c>
       <c r="C284" s="2" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="D284" s="2" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="E284" s="2" t="s">
         <v>3353</v>
@@ -35143,12 +35143,12 @@
         <v>125</v>
       </c>
       <c r="T289" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="U289" s="2"/>
       <c r="V289" s="2"/>
       <c r="W289" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="X289" s="2" t="s">
         <v>92</v>
@@ -35894,7 +35894,7 @@
         <v>105</v>
       </c>
       <c r="C299" s="2" t="s">
-        <v>3850</v>
+        <v>3849</v>
       </c>
       <c r="D299" s="2" t="s">
         <v>212</v>
@@ -36288,7 +36288,7 @@
         <v>105</v>
       </c>
       <c r="C304" s="2" t="s">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="D304" s="2" t="s">
         <v>1776</v>
@@ -36602,10 +36602,10 @@
         <v>105</v>
       </c>
       <c r="C308" s="2" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
       <c r="D308" s="2" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
       <c r="E308" s="2" t="s">
         <v>2878</v>
@@ -36765,7 +36765,7 @@
         <v>797</v>
       </c>
       <c r="D310" s="2" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="E310" s="2" t="s">
         <v>796</v>
@@ -37072,16 +37072,16 @@
         <v>1</v>
       </c>
       <c r="C314" s="2" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="D314" s="2" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="E314" s="2" t="s">
         <v>2384</v>
       </c>
       <c r="F314" s="2" t="s">
-        <v>3887</v>
+        <v>3886</v>
       </c>
       <c r="G314" s="2">
         <v>42851</v>
@@ -37150,7 +37150,7 @@
         <v>105</v>
       </c>
       <c r="C315" s="2" t="s">
-        <v>3824</v>
+        <v>3823</v>
       </c>
       <c r="D315" s="2" t="s">
         <v>533</v>
@@ -37226,7 +37226,7 @@
         <v>105</v>
       </c>
       <c r="C316" s="2" t="s">
-        <v>3836</v>
+        <v>3835</v>
       </c>
       <c r="D316" s="2" t="s">
         <v>181</v>
@@ -37460,10 +37460,10 @@
         <v>1</v>
       </c>
       <c r="C319" s="2" t="s">
-        <v>3855</v>
+        <v>3854</v>
       </c>
       <c r="D319" s="2" t="s">
-        <v>3855</v>
+        <v>3854</v>
       </c>
       <c r="E319" s="2" t="s">
         <v>2544</v>
@@ -37536,7 +37536,7 @@
         <v>105</v>
       </c>
       <c r="C320" s="2" t="s">
-        <v>3861</v>
+        <v>3860</v>
       </c>
       <c r="D320" s="2" t="s">
         <v>189</v>
@@ -37614,7 +37614,7 @@
         <v>105</v>
       </c>
       <c r="C321" s="2" t="s">
-        <v>3863</v>
+        <v>3862</v>
       </c>
       <c r="D321" s="2" t="s">
         <v>174</v>
@@ -38568,7 +38568,7 @@
         <v>105</v>
       </c>
       <c r="C333" s="2" t="s">
-        <v>3823</v>
+        <v>3822</v>
       </c>
       <c r="D333" s="2" t="s">
         <v>611</v>
@@ -38646,7 +38646,7 @@
         <v>105</v>
       </c>
       <c r="C334" s="2" t="s">
-        <v>3826</v>
+        <v>3825</v>
       </c>
       <c r="D334" s="2" t="s">
         <v>524</v>
@@ -38724,7 +38724,7 @@
         <v>105</v>
       </c>
       <c r="C335" s="2" t="s">
-        <v>3852</v>
+        <v>3851</v>
       </c>
       <c r="D335" s="2" t="s">
         <v>300</v>
@@ -39744,7 +39744,7 @@
         <v>105</v>
       </c>
       <c r="C348" s="2" t="s">
-        <v>3857</v>
+        <v>3856</v>
       </c>
       <c r="D348" s="2" t="s">
         <v>1131</v>
@@ -40614,7 +40614,7 @@
         <v>105</v>
       </c>
       <c r="C359" s="2" t="s">
-        <v>3822</v>
+        <v>3821</v>
       </c>
       <c r="D359" s="2" t="s">
         <v>701</v>
@@ -40690,7 +40690,7 @@
         <v>1</v>
       </c>
       <c r="C360" s="2" t="s">
-        <v>3831</v>
+        <v>3830</v>
       </c>
       <c r="D360" s="2" t="s">
         <v>35</v>
@@ -40766,7 +40766,7 @@
         <v>105</v>
       </c>
       <c r="C361" s="2" t="s">
-        <v>3832</v>
+        <v>3831</v>
       </c>
       <c r="D361" s="2" t="s">
         <v>329</v>
@@ -40924,7 +40924,7 @@
         <v>105</v>
       </c>
       <c r="C363" s="2" t="s">
-        <v>3862</v>
+        <v>3861</v>
       </c>
       <c r="D363" s="2" t="s">
         <v>195</v>
@@ -41636,7 +41636,7 @@
         <v>105</v>
       </c>
       <c r="C372" s="2" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="D372" s="2" t="s">
         <v>274</v>
@@ -41718,7 +41718,7 @@
         <v>105</v>
       </c>
       <c r="C373" s="2" t="s">
-        <v>3891</v>
+        <v>3890</v>
       </c>
       <c r="D373" s="2" t="s">
         <v>133</v>
@@ -41798,7 +41798,7 @@
         <v>1</v>
       </c>
       <c r="C374" s="2" t="s">
-        <v>3838</v>
+        <v>3837</v>
       </c>
       <c r="D374" s="2" t="s">
         <v>37</v>
@@ -41956,7 +41956,7 @@
         <v>105</v>
       </c>
       <c r="C376" s="2" t="s">
-        <v>3840</v>
+        <v>3839</v>
       </c>
       <c r="D376" s="2" t="s">
         <v>1101</v>
@@ -42034,7 +42034,7 @@
         <v>105</v>
       </c>
       <c r="C377" s="2" t="s">
-        <v>3843</v>
+        <v>3842</v>
       </c>
       <c r="D377" s="2" t="s">
         <v>3223</v>
@@ -42781,12 +42781,12 @@
         <v>125</v>
       </c>
       <c r="T386" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="U386" s="2"/>
       <c r="V386" s="2"/>
       <c r="W386" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="X386" s="2" t="s">
         <v>92</v>
@@ -42810,7 +42810,7 @@
         <v>105</v>
       </c>
       <c r="C387" s="2" t="s">
-        <v>3820</v>
+        <v>3899</v>
       </c>
       <c r="D387" s="2" t="s">
         <v>858</v>
@@ -43270,7 +43270,7 @@
         <v>105</v>
       </c>
       <c r="C393" s="2" t="s">
-        <v>3871</v>
+        <v>3870</v>
       </c>
       <c r="D393" s="2" t="s">
         <v>1123</v>
@@ -43557,12 +43557,12 @@
         <v>125</v>
       </c>
       <c r="T396" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="U396" s="2"/>
       <c r="V396" s="2"/>
       <c r="W396" s="2" t="s">
-        <v>3890</v>
+        <v>3889</v>
       </c>
       <c r="X396" s="2" t="s">
         <v>92</v>
@@ -43586,7 +43586,7 @@
         <v>105</v>
       </c>
       <c r="C397" s="2" t="s">
-        <v>3821</v>
+        <v>3820</v>
       </c>
       <c r="D397" s="2" t="s">
         <v>2605</v>
@@ -43662,10 +43662,10 @@
         <v>105</v>
       </c>
       <c r="C398" s="2" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="D398" s="2" t="s">
-        <v>3844</v>
+        <v>3843</v>
       </c>
       <c r="E398" s="2" t="s">
         <v>1807</v>
@@ -43738,7 +43738,7 @@
         <v>105</v>
       </c>
       <c r="C399" s="2" t="s">
-        <v>3845</v>
+        <v>3844</v>
       </c>
       <c r="D399" s="2" t="s">
         <v>875</v>
@@ -44134,7 +44134,7 @@
         <v>1</v>
       </c>
       <c r="C404" s="2" t="s">
-        <v>3839</v>
+        <v>3838</v>
       </c>
       <c r="D404" s="2" t="s">
         <v>3624</v>
@@ -44216,7 +44216,7 @@
         <v>105</v>
       </c>
       <c r="C405" s="2" t="s">
-        <v>3841</v>
+        <v>3840</v>
       </c>
       <c r="D405" s="2" t="s">
         <v>265</v>
@@ -44610,7 +44610,7 @@
         <v>105</v>
       </c>
       <c r="C410" s="2" t="s">
-        <v>3827</v>
+        <v>3826</v>
       </c>
       <c r="D410" s="2" t="s">
         <v>1547</v>
@@ -44688,7 +44688,7 @@
         <v>105</v>
       </c>
       <c r="C411" s="2" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="D411" s="2" t="s">
         <v>150</v>
@@ -44770,7 +44770,7 @@
         <v>105</v>
       </c>
       <c r="C412" s="2" t="s">
-        <v>3847</v>
+        <v>3846</v>
       </c>
       <c r="D412" s="2" t="s">
         <v>3002</v>
@@ -45244,10 +45244,10 @@
         <v>105</v>
       </c>
       <c r="C418" s="2" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="D418" s="2" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="E418" s="2" t="s">
         <v>2061</v>
@@ -45476,7 +45476,7 @@
         <v>1</v>
       </c>
       <c r="C421" s="2" t="s">
-        <v>3830</v>
+        <v>3829</v>
       </c>
       <c r="D421" s="2" t="s">
         <v>21</v>
@@ -45636,7 +45636,7 @@
         <v>105</v>
       </c>
       <c r="C423" s="2" t="s">
-        <v>3865</v>
+        <v>3864</v>
       </c>
       <c r="D423" s="2" t="s">
         <v>3295</v>
@@ -45798,7 +45798,7 @@
         <v>105</v>
       </c>
       <c r="C425" s="2" t="s">
-        <v>3858</v>
+        <v>3857</v>
       </c>
       <c r="D425" s="2" t="s">
         <v>2215</v>
@@ -45952,7 +45952,7 @@
         <v>105</v>
       </c>
       <c r="C427" s="2" t="s">
-        <v>3870</v>
+        <v>3869</v>
       </c>
       <c r="D427" s="2" t="s">
         <v>2313</v>
@@ -46032,7 +46032,7 @@
         <v>105</v>
       </c>
       <c r="C428" s="2" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="D428" s="2" t="s">
         <v>158</v>
@@ -46190,7 +46190,7 @@
         <v>105</v>
       </c>
       <c r="C430" s="2" t="s">
-        <v>3829</v>
+        <v>3828</v>
       </c>
       <c r="D430" s="2" t="s">
         <v>357</v>
@@ -46505,7 +46505,7 @@
         <v>1055</v>
       </c>
       <c r="D434" s="2" t="s">
-        <v>3895</v>
+        <v>3894</v>
       </c>
       <c r="E434" s="2" t="s">
         <v>1054</v>
@@ -46732,10 +46732,10 @@
         <v>105</v>
       </c>
       <c r="C437" s="2" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="D437" s="2" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="E437" s="2" t="s">
         <v>2248</v>
@@ -46888,10 +46888,10 @@
         <v>105</v>
       </c>
       <c r="C439" s="2" t="s">
+        <v>3865</v>
+      </c>
+      <c r="D439" s="2" t="s">
         <v>3866</v>
-      </c>
-      <c r="D439" s="2" t="s">
-        <v>3867</v>
       </c>
       <c r="E439" s="2" t="s">
         <v>1694</v>
@@ -46969,7 +46969,7 @@
         <v>2255</v>
       </c>
       <c r="D440" s="2" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="E440" s="2" t="s">
         <v>2254</v>
@@ -47042,10 +47042,10 @@
         <v>1</v>
       </c>
       <c r="C441" s="2" t="s">
-        <v>3869</v>
+        <v>3868</v>
       </c>
       <c r="D441" s="2" t="s">
-        <v>3868</v>
+        <v>3867</v>
       </c>
       <c r="E441" s="2" t="s">
         <v>2346</v>
@@ -47196,7 +47196,7 @@
         <v>105</v>
       </c>
       <c r="C443" s="2" t="s">
-        <v>3859</v>
+        <v>3858</v>
       </c>
       <c r="D443" s="2" t="s">
         <v>1004</v>
@@ -47351,23 +47351,23 @@
   <conditionalFormatting sqref="C10">
     <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="C83:C84">
+    <cfRule type="duplicateValues" dxfId="7" priority="1"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="D1 D231:D266 D3:D75 D77:D79 C76 D81:D82 C80 D85:D193 D441:D443 D268 D270:D271 D273:D279 D281:D297 D299:D304 D306:D322 D324:D402 D404:D416 D418:D428 D431:D435 D437:D439 D195:D228">
-    <cfRule type="duplicateValues" dxfId="7" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F1:F444">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N56 N58:N75 N371:N444">
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="3" priority="6" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",N1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X1:AD1 D1 F1:L1 N1">
-    <cfRule type="duplicateValues" dxfId="3" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C83:C84">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="7"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>